<commit_message>
Replace histogram by pie chart in division_compare
</commit_message>
<xml_diff>
--- a/Result_6.xlsx
+++ b/Result_6.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1334,7 +1334,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1355,11 +1355,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1404,16 +1399,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1436,8 +1427,8 @@
   </sheetPr>
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N53" activeCellId="0" sqref="N53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N37" activeCellId="0" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1715,7 +1706,7 @@
         <v>9</v>
       </c>
       <c r="J6" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>10</v>
@@ -1731,7 +1722,7 @@
       </c>
       <c r="O6" s="1" t="n">
         <f aca="false">ROUND(SUM(F6*4,G6*4,H6*4,I6*3,J6*3,K6*3,L6*2,M6*2,N6*2)/27,2)</f>
-        <v>8.59</v>
+        <v>8.04</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,14 +1763,14 @@
         <v>9</v>
       </c>
       <c r="M7" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N7" s="1" t="n">
         <v>9</v>
       </c>
       <c r="O7" s="1" t="n">
         <f aca="false">ROUND(SUM(F7*4,G7*4,H7*4,I7*3,J7*3,K7*3,L7*2,M7*2,N7*2)/27,2)</f>
-        <v>6.59</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,17 +1856,17 @@
         <v>0</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M9" s="1" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N9" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="O9" s="1" t="n">
         <f aca="false">ROUND(SUM(F9*4,G9*4,H9*4,I9*3,J9*3,K9*3,L9*2,M9*2,N9*2)/27,2)</f>
-        <v>4.7</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1952,26 +1943,26 @@
         <v>6</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K11" s="1" t="n">
         <v>9</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N11" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O11" s="1" t="n">
         <f aca="false">ROUND(SUM(F11*4,G11*4,H11*4,I11*3,J11*3,K11*3,L11*2,M11*2,N11*2)/27,2)</f>
-        <v>7.89</v>
+        <v>5.89</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1991,7 +1982,7 @@
         <v>38</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G12" s="1" t="n">
         <v>9</v>
@@ -2019,7 +2010,7 @@
       </c>
       <c r="O12" s="1" t="n">
         <f aca="false">ROUND(SUM(F12*4,G12*4,H12*4,I12*3,J12*3,K12*3,L12*2,M12*2,N12*2)/27,2)</f>
-        <v>8.3</v>
+        <v>7.56</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2243,23 +2234,23 @@
         <v>8</v>
       </c>
       <c r="J17" s="1" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K17" s="1" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="L17" s="1" t="n">
         <v>9</v>
       </c>
       <c r="M17" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O17" s="1" t="n">
         <f aca="false">ROUND(SUM(F17*4,G17*4,H17*4,I17*3,J17*3,K17*3,L17*2,M17*2,N17*2)/27,2)</f>
-        <v>6.89</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2345,7 +2336,7 @@
         <v>8</v>
       </c>
       <c r="L19" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M19" s="1" t="n">
         <v>9</v>
@@ -2355,7 +2346,7 @@
       </c>
       <c r="O19" s="1" t="n">
         <f aca="false">ROUND(SUM(F19*4,G19*4,H19*4,I19*3,J19*3,K19*3,L19*2,M19*2,N19*2)/27,2)</f>
-        <v>7.3</v>
+        <v>6.93</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2381,7 +2372,7 @@
         <v>6</v>
       </c>
       <c r="H20" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I20" s="1" t="n">
         <v>8</v>
@@ -2396,14 +2387,14 @@
         <v>9</v>
       </c>
       <c r="M20" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N20" s="1" t="n">
         <v>9</v>
       </c>
       <c r="O20" s="1" t="n">
         <f aca="false">ROUND(SUM(F20*4,G20*4,H20*4,I20*3,J20*3,K20*3,L20*2,M20*2,N20*2)/27,2)</f>
-        <v>7.3</v>
+        <v>6.48</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2435,7 +2426,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="1" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K21" s="1" t="n">
         <v>7</v>
@@ -2447,11 +2438,11 @@
         <v>0</v>
       </c>
       <c r="N21" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O21" s="1" t="n">
         <f aca="false">ROUND(SUM(F21*4,G21*4,H21*4,I21*3,J21*3,K21*3,L21*2,M21*2,N21*2)/27,2)</f>
-        <v>3.44</v>
+        <v>2.26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2480,7 +2471,7 @@
         <v>8</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J22" s="1" t="n">
         <v>6</v>
@@ -2499,7 +2490,7 @@
       </c>
       <c r="O22" s="1" t="n">
         <f aca="false">ROUND(SUM(F22*4,G22*4,H22*4,I22*3,J22*3,K22*3,L22*2,M22*2,N22*2)/27,2)</f>
-        <v>8.26</v>
+        <v>7.59</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2694,7 +2685,7 @@
         <v>8.78</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>6</v>
       </c>
@@ -2723,13 +2714,13 @@
         <v>0</v>
       </c>
       <c r="J27" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K27" s="1" t="n">
         <v>9</v>
       </c>
       <c r="L27" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="M27" s="1" t="n">
         <v>0</v>
@@ -2739,10 +2730,10 @@
       </c>
       <c r="O27" s="1" t="n">
         <f aca="false">ROUND(SUM(F27*4,G27*4,H27*4,I27*3,J27*3,K27*3,L27*2,M27*2,N27*2)/27,2)</f>
-        <v>4.89</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>6</v>
       </c>
@@ -2790,7 +2781,7 @@
         <v>8.37</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>6</v>
       </c>
@@ -2838,7 +2829,7 @@
         <v>7.78</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>6</v>
       </c>
@@ -2864,7 +2855,7 @@
         <v>7</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J30" s="1" t="n">
         <v>7</v>
@@ -2879,14 +2870,14 @@
         <v>6</v>
       </c>
       <c r="N30" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O30" s="1" t="n">
         <f aca="false">ROUND(SUM(F30*4,G30*4,H30*4,I30*3,J30*3,K30*3,L30*2,M30*2,N30*2)/27,2)</f>
-        <v>7.04</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.19</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>6</v>
       </c>
@@ -2934,7 +2925,7 @@
         <v>7.15</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>6</v>
       </c>
@@ -2982,7 +2973,7 @@
         <v>8.04</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>6</v>
       </c>
@@ -3030,7 +3021,7 @@
         <v>8.63</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>6</v>
       </c>
@@ -3068,17 +3059,17 @@
         <v>9</v>
       </c>
       <c r="M34" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="N34" s="1" t="n">
         <v>0</v>
       </c>
       <c r="O34" s="1" t="n">
         <f aca="false">ROUND(SUM(F34*4,G34*4,H34*4,I34*3,J34*3,K34*3,L34*2,M34*2,N34*2)/27,2)</f>
-        <v>6.89</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.52</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>6</v>
       </c>
@@ -3126,7 +3117,7 @@
         <v>8.37</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>6</v>
       </c>
@@ -3174,7 +3165,7 @@
         <v>8.56</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <v>6</v>
       </c>
@@ -3194,7 +3185,7 @@
         <v>5</v>
       </c>
       <c r="G37" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H37" s="1" t="n">
         <v>7</v>
@@ -3203,26 +3194,26 @@
         <v>8</v>
       </c>
       <c r="J37" s="1" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K37" s="1" t="n">
         <v>6</v>
       </c>
       <c r="L37" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M37" s="1" t="n">
         <v>8</v>
       </c>
       <c r="N37" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="O37" s="1" t="n">
         <f aca="false">ROUND(SUM(F37*4,G37*4,H37*4,I37*3,J37*3,K37*3,L37*2,M37*2,N37*2)/27,2)</f>
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.19</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <v>6</v>
       </c>
@@ -3245,7 +3236,7 @@
         <v>8</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I38" s="1" t="n">
         <v>9</v>
@@ -3267,10 +3258,10 @@
       </c>
       <c r="O38" s="1" t="n">
         <f aca="false">ROUND(SUM(F38*4,G38*4,H38*4,I38*3,J38*3,K38*3,L38*2,M38*2,N38*2)/27,2)</f>
-        <v>8.07</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.48</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>6</v>
       </c>
@@ -3318,7 +3309,7 @@
         <v>8.41</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>6</v>
       </c>
@@ -3366,7 +3357,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <v>6</v>
       </c>
@@ -3414,7 +3405,7 @@
         <v>7.93</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>6</v>
       </c>
@@ -3462,7 +3453,7 @@
         <v>8.59</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>6</v>
       </c>
@@ -3510,7 +3501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <v>6</v>
       </c>
@@ -3545,7 +3536,7 @@
         <v>6</v>
       </c>
       <c r="L44" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="M44" s="1" t="n">
         <v>9</v>
@@ -3555,10 +3546,10 @@
       </c>
       <c r="O44" s="1" t="n">
         <f aca="false">ROUND(SUM(F44*4,G44*4,H44*4,I44*3,J44*3,K44*3,L44*2,M44*2,N44*2)/27,2)</f>
-        <v>7.56</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <v>6</v>
       </c>
@@ -3606,7 +3597,7 @@
         <v>8.11</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <v>6</v>
       </c>
@@ -3654,7 +3645,7 @@
         <v>8.85</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <v>6</v>
       </c>
@@ -3674,7 +3665,7 @@
         <v>8</v>
       </c>
       <c r="G47" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H47" s="1" t="n">
         <v>5</v>
@@ -3699,10 +3690,10 @@
       </c>
       <c r="O47" s="1" t="n">
         <f aca="false">ROUND(SUM(F47*4,G47*4,H47*4,I47*3,J47*3,K47*3,L47*2,M47*2,N47*2)/27,2)</f>
-        <v>7.89</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>6</v>
       </c>
@@ -3725,7 +3716,7 @@
         <v>8</v>
       </c>
       <c r="H48" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I48" s="1" t="n">
         <v>8</v>
@@ -3747,10 +3738,10 @@
       </c>
       <c r="O48" s="1" t="n">
         <f aca="false">ROUND(SUM(F48*4,G48*4,H48*4,I48*3,J48*3,K48*3,L48*2,M48*2,N48*2)/27,2)</f>
-        <v>7.96</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.22</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>6</v>
       </c>
@@ -3798,7 +3789,7 @@
         <v>8.22</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>6</v>
       </c>
@@ -3846,7 +3837,7 @@
         <v>6.78</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
         <v>6</v>
       </c>
@@ -3863,10 +3854,10 @@
         <v>116</v>
       </c>
       <c r="F51" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G51" s="1" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H51" s="1" t="n">
         <v>8</v>
@@ -3891,10 +3882,10 @@
       </c>
       <c r="O51" s="1" t="n">
         <f aca="false">ROUND(SUM(F51*4,G51*4,H51*4,I51*3,J51*3,K51*3,L51*2,M51*2,N51*2)/27,2)</f>
-        <v>7.33</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
         <v>6</v>
       </c>
@@ -3942,7 +3933,7 @@
         <v>6.37</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <v>6</v>
       </c>
@@ -3990,7 +3981,7 @@
         <v>8.3</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
         <v>6</v>
       </c>
@@ -4038,7 +4029,7 @@
         <v>8.11</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <v>6</v>
       </c>
@@ -4055,7 +4046,7 @@
         <v>124</v>
       </c>
       <c r="F55" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G55" s="1" t="n">
         <v>9</v>
@@ -4083,10 +4074,10 @@
       </c>
       <c r="O55" s="1" t="n">
         <f aca="false">ROUND(SUM(F55*4,G55*4,H55*4,I55*3,J55*3,K55*3,L55*2,M55*2,N55*2)/27,2)</f>
-        <v>7.07</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <v>6</v>
       </c>
@@ -4134,7 +4125,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
         <v>6</v>
       </c>
@@ -4151,7 +4142,7 @@
         <v>128</v>
       </c>
       <c r="F57" s="1" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G57" s="1" t="n">
         <v>8</v>
@@ -4179,10 +4170,10 @@
       </c>
       <c r="O57" s="1" t="n">
         <f aca="false">ROUND(SUM(F57*4,G57*4,H57*4,I57*3,J57*3,K57*3,L57*2,M57*2,N57*2)/27,2)</f>
-        <v>7.37</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.19</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
         <v>6</v>
       </c>
@@ -4230,7 +4221,7 @@
         <v>8.22</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
         <v>6</v>
       </c>
@@ -4278,7 +4269,7 @@
         <v>7.56</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
         <v>6</v>
       </c>
@@ -4326,7 +4317,7 @@
         <v>6.07</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
         <v>6</v>
       </c>
@@ -4392,8 +4383,8 @@
   </sheetPr>
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L60" activeCellId="0" sqref="L60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N16" activeCellId="0" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5008,10 +4999,10 @@
         <v>4</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L13" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M13" s="1" t="n">
         <v>9</v>
@@ -5021,7 +5012,7 @@
       </c>
       <c r="O13" s="1" t="n">
         <f aca="false">ROUND(SUM(F13*4,G13*4,H13*4,I13*3,J13*3,K13*3,L13*2,M13*2,N13*2)/27,2)</f>
-        <v>5.15</v>
+        <v>3.74</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5395,17 +5386,17 @@
         <v>7</v>
       </c>
       <c r="L21" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M21" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N21" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O21" s="1" t="n">
         <f aca="false">ROUND(SUM(F21*4,G21*4,H21*4,I21*3,J21*3,K21*3,L21*2,M21*2,N21*2)/27,2)</f>
-        <v>3.44</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5488,7 +5479,7 @@
         <v>9</v>
       </c>
       <c r="K23" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L23" s="1" t="n">
         <v>10</v>
@@ -5501,7 +5492,7 @@
       </c>
       <c r="O23" s="1" t="n">
         <f aca="false">ROUND(SUM(F23*4,G23*4,H23*4,I23*3,J23*3,K23*3,L23*2,M23*2,N23*2)/27,2)</f>
-        <v>8.96</v>
+        <v>9.07</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5680,7 +5671,7 @@
         <v>9</v>
       </c>
       <c r="K27" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L27" s="1" t="n">
         <v>9</v>
@@ -5693,7 +5684,7 @@
       </c>
       <c r="O27" s="1" t="n">
         <f aca="false">ROUND(SUM(F27*4,G27*4,H27*4,I27*3,J27*3,K27*3,L27*2,M27*2,N27*2)/27,2)</f>
-        <v>5.63</v>
+        <v>5.07</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5776,7 +5767,7 @@
         <v>10</v>
       </c>
       <c r="K29" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L29" s="1" t="n">
         <v>10</v>
@@ -5789,7 +5780,7 @@
       </c>
       <c r="O29" s="1" t="n">
         <f aca="false">ROUND(SUM(F29*4,G29*4,H29*4,I29*3,J29*3,K29*3,L29*2,M29*2,N29*2)/27,2)</f>
-        <v>8.56</v>
+        <v>8.67</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5812,16 +5803,16 @@
         <v>5</v>
       </c>
       <c r="G30" s="1" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H30" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I30" s="1" t="n">
         <v>9</v>
       </c>
       <c r="J30" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K30" s="1" t="n">
         <v>8</v>
@@ -5833,11 +5824,11 @@
         <v>6</v>
       </c>
       <c r="N30" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="O30" s="1" t="n">
         <f aca="false">ROUND(SUM(F30*4,G30*4,H30*4,I30*3,J30*3,K30*3,L30*2,M30*2,N30*2)/27,2)</f>
-        <v>7.04</v>
+        <v>3.96</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6004,13 +5995,13 @@
         <v>8</v>
       </c>
       <c r="G34" s="1" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H34" s="1" t="n">
         <v>7</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J34" s="1" t="n">
         <v>5</v>
@@ -6029,7 +6020,7 @@
       </c>
       <c r="O34" s="1" t="n">
         <f aca="false">ROUND(SUM(F34*4,G34*4,H34*4,I34*3,J34*3,K34*3,L34*2,M34*2,N34*2)/27,2)</f>
-        <v>6.89</v>
+        <v>5.22</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6448,7 +6439,7 @@
         <v>6</v>
       </c>
       <c r="K43" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L43" s="1" t="n">
         <v>9</v>
@@ -6461,7 +6452,7 @@
       </c>
       <c r="O43" s="1" t="n">
         <f aca="false">ROUND(SUM(F43*4,G43*4,H43*4,I43*3,J43*3,K43*3,L43*2,M43*2,N43*2)/27,2)</f>
-        <v>8</v>
+        <v>7.78</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6532,10 +6523,10 @@
         <v>10</v>
       </c>
       <c r="G45" s="1" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H45" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I45" s="1" t="n">
         <v>6</v>
@@ -6557,7 +6548,7 @@
       </c>
       <c r="O45" s="1" t="n">
         <f aca="false">ROUND(SUM(F45*4,G45*4,H45*4,I45*3,J45*3,K45*3,L45*2,M45*2,N45*2)/27,2)</f>
-        <v>6.15</v>
+        <v>3.78</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6778,10 +6769,10 @@
         <v>6</v>
       </c>
       <c r="I50" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J50" s="1" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K50" s="1" t="n">
         <v>0</v>
@@ -6797,7 +6788,7 @@
       </c>
       <c r="O50" s="1" t="n">
         <f aca="false">ROUND(SUM(F50*4,G50*4,H50*4,I50*3,J50*3,K50*3,L50*2,M50*2,N50*2)/27,2)</f>
-        <v>4.56</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6925,7 +6916,7 @@
         <v>7</v>
       </c>
       <c r="J53" s="1" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="K53" s="1" t="n">
         <v>7</v>
@@ -6941,7 +6932,7 @@
       </c>
       <c r="O53" s="1" t="n">
         <f aca="false">ROUND(SUM(F53*4,G53*4,H53*4,I53*3,J53*3,K53*3,L53*2,M53*2,N53*2)/27,2)</f>
-        <v>7.93</v>
+        <v>7.26</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7018,7 +7009,7 @@
         <v>8</v>
       </c>
       <c r="I55" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J55" s="1" t="n">
         <v>5</v>
@@ -7037,7 +7028,7 @@
       </c>
       <c r="O55" s="1" t="n">
         <f aca="false">ROUND(SUM(F55*4,G55*4,H55*4,I55*3,J55*3,K55*3,L55*2,M55*2,N55*2)/27,2)</f>
-        <v>7.07</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7261,10 +7252,10 @@
         <v>5</v>
       </c>
       <c r="J60" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K60" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L60" s="1" t="n">
         <v>7</v>
@@ -7277,7 +7268,7 @@
       </c>
       <c r="O60" s="1" t="n">
         <f aca="false">ROUND(SUM(F60*4,G60*4,H60*4,I60*3,J60*3,K60*3,L60*2,M60*2,N60*2)/27,2)</f>
-        <v>6.15</v>
+        <v>5.26</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7346,8 +7337,8 @@
   </sheetPr>
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M57" activeCellId="0" sqref="M57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L32" activeCellId="0" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7628,7 +7619,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>9</v>
@@ -7653,7 +7644,7 @@
       </c>
       <c r="O6" s="1" t="n">
         <f aca="false">ROUND(SUM(F6*4,G6*4,H6*4,I6*3,J6*3,K6*3,L6*2,M6*2,N6*2)/27,2)</f>
-        <v>7.56</v>
+        <v>6.22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7916,7 +7907,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>10</v>
@@ -7941,7 +7932,7 @@
       </c>
       <c r="O12" s="1" t="n">
         <f aca="false">ROUND(SUM(F12*4,G12*4,H12*4,I12*3,J12*3,K12*3,L12*2,M12*2,N12*2)/27,2)</f>
-        <v>6.41</v>
+        <v>5.81</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7970,16 +7961,16 @@
         <v>4</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>5</v>
       </c>
       <c r="L13" s="1" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M13" s="1" t="n">
         <v>9</v>
@@ -7989,7 +7980,7 @@
       </c>
       <c r="O13" s="1" t="n">
         <f aca="false">ROUND(SUM(F13*4,G13*4,H13*4,I13*3,J13*3,K13*3,L13*2,M13*2,N13*2)/27,2)</f>
-        <v>4.96</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8012,7 +8003,7 @@
         <v>4</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>7</v>
@@ -8024,7 +8015,7 @@
         <v>9</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L14" s="1" t="n">
         <v>4</v>
@@ -8037,7 +8028,7 @@
       </c>
       <c r="O14" s="1" t="n">
         <f aca="false">ROUND(SUM(F14*4,G14*4,H14*4,I14*3,J14*3,K14*3,L14*2,M14*2,N14*2)/27,2)</f>
-        <v>6.67</v>
+        <v>6.85</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8159,7 +8150,7 @@
         <v>8</v>
       </c>
       <c r="H17" s="1" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I17" s="1" t="n">
         <v>9</v>
@@ -8181,7 +8172,7 @@
       </c>
       <c r="O17" s="1" t="n">
         <f aca="false">ROUND(SUM(F17*4,G17*4,H17*4,I17*3,J17*3,K17*3,L17*2,M17*2,N17*2)/27,2)</f>
-        <v>6.96</v>
+        <v>6.07</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8216,7 +8207,7 @@
         <v>8</v>
       </c>
       <c r="K18" s="1" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="L18" s="1" t="n">
         <v>4</v>
@@ -8229,7 +8220,7 @@
       </c>
       <c r="O18" s="1" t="n">
         <f aca="false">ROUND(SUM(F18*4,G18*4,H18*4,I18*3,J18*3,K18*3,L18*2,M18*2,N18*2)/27,2)</f>
-        <v>7.04</v>
+        <v>6.37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8252,7 +8243,7 @@
         <v>9</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>6</v>
@@ -8277,7 +8268,7 @@
       </c>
       <c r="O19" s="1" t="n">
         <f aca="false">ROUND(SUM(F19*4,G19*4,H19*4,I19*3,J19*3,K19*3,L19*2,M19*2,N19*2)/27,2)</f>
-        <v>8.04</v>
+        <v>7.59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8357,7 +8348,7 @@
         <v>10</v>
       </c>
       <c r="J21" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K21" s="1" t="n">
         <v>7</v>
@@ -8373,7 +8364,7 @@
       </c>
       <c r="O21" s="1" t="n">
         <f aca="false">ROUND(SUM(F21*4,G21*4,H21*4,I21*3,J21*3,K21*3,L21*2,M21*2,N21*2)/27,2)</f>
-        <v>8.37</v>
+        <v>7.81</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8885,13 +8876,13 @@
         <v>8</v>
       </c>
       <c r="J32" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K32" s="1" t="n">
         <v>5</v>
       </c>
       <c r="L32" s="1" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M32" s="1" t="n">
         <v>0</v>
@@ -8901,7 +8892,7 @@
       </c>
       <c r="O32" s="1" t="n">
         <f aca="false">ROUND(SUM(F32*4,G32*4,H32*4,I32*3,J32*3,K32*3,L32*2,M32*2,N32*2)/27,2)</f>
-        <v>6.48</v>
+        <v>5.52</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9029,7 +9020,7 @@
         <v>9</v>
       </c>
       <c r="J35" s="1" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K35" s="1" t="n">
         <v>8</v>
@@ -9045,7 +9036,7 @@
       </c>
       <c r="O35" s="1" t="n">
         <f aca="false">ROUND(SUM(F35*4,G35*4,H35*4,I35*3,J35*3,K35*3,L35*2,M35*2,N35*2)/27,2)</f>
-        <v>8.26</v>
+        <v>8.7</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9074,7 +9065,7 @@
         <v>5</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J36" s="1" t="n">
         <v>5</v>
@@ -9093,7 +9084,7 @@
       </c>
       <c r="O36" s="1" t="n">
         <f aca="false">ROUND(SUM(F36*4,G36*4,H36*4,I36*3,J36*3,K36*3,L36*2,M36*2,N36*2)/27,2)</f>
-        <v>6.56</v>
+        <v>6.44</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9122,7 +9113,7 @@
         <v>9</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J37" s="1" t="n">
         <v>9</v>
@@ -9141,7 +9132,7 @@
       </c>
       <c r="O37" s="1" t="n">
         <f aca="false">ROUND(SUM(F37*4,G37*4,H37*4,I37*3,J37*3,K37*3,L37*2,M37*2,N37*2)/27,2)</f>
-        <v>6.67</v>
+        <v>6.56</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9221,7 +9212,7 @@
         <v>5</v>
       </c>
       <c r="J39" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K39" s="1" t="n">
         <v>8</v>
@@ -9237,7 +9228,7 @@
       </c>
       <c r="O39" s="1" t="n">
         <f aca="false">ROUND(SUM(F39*4,G39*4,H39*4,I39*3,J39*3,K39*3,L39*2,M39*2,N39*2)/27,2)</f>
-        <v>6.89</v>
+        <v>6.11</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9260,7 +9251,7 @@
         <v>7</v>
       </c>
       <c r="G40" s="1" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H40" s="1" t="n">
         <v>7</v>
@@ -9285,7 +9276,7 @@
       </c>
       <c r="O40" s="1" t="n">
         <f aca="false">ROUND(SUM(F40*4,G40*4,H40*4,I40*3,J40*3,K40*3,L40*2,M40*2,N40*2)/27,2)</f>
-        <v>6.93</v>
+        <v>7.37</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9365,7 +9356,7 @@
         <v>5</v>
       </c>
       <c r="J42" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K42" s="1" t="n">
         <v>8</v>
@@ -9381,7 +9372,7 @@
       </c>
       <c r="O42" s="1" t="n">
         <f aca="false">ROUND(SUM(F42*4,G42*4,H42*4,I42*3,J42*3,K42*3,L42*2,M42*2,N42*2)/27,2)</f>
-        <v>8.07</v>
+        <v>7.74</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9461,7 +9452,7 @@
         <v>7</v>
       </c>
       <c r="J44" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K44" s="1" t="n">
         <v>6</v>
@@ -9477,7 +9468,7 @@
       </c>
       <c r="O44" s="1" t="n">
         <f aca="false">ROUND(SUM(F44*4,G44*4,H44*4,I44*3,J44*3,K44*3,L44*2,M44*2,N44*2)/27,2)</f>
-        <v>7.56</v>
+        <v>8.11</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9701,7 +9692,7 @@
         <v>9</v>
       </c>
       <c r="J49" s="1" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="K49" s="1" t="n">
         <v>8</v>
@@ -9717,7 +9708,7 @@
       </c>
       <c r="O49" s="1" t="n">
         <f aca="false">ROUND(SUM(F49*4,G49*4,H49*4,I49*3,J49*3,K49*3,L49*2,M49*2,N49*2)/27,2)</f>
-        <v>8.22</v>
+        <v>8.56</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9989,7 +9980,7 @@
         <v>8</v>
       </c>
       <c r="J55" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K55" s="1" t="n">
         <v>4</v>
@@ -10005,7 +9996,7 @@
       </c>
       <c r="O55" s="1" t="n">
         <f aca="false">ROUND(SUM(F55*4,G55*4,H55*4,I55*3,J55*3,K55*3,L55*2,M55*2,N55*2)/27,2)</f>
-        <v>7.07</v>
+        <v>7.63</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10226,7 +10217,7 @@
         <v>9</v>
       </c>
       <c r="I60" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J60" s="1" t="n">
         <v>8</v>
@@ -10245,7 +10236,7 @@
       </c>
       <c r="O60" s="1" t="n">
         <f aca="false">ROUND(SUM(F60*4,G60*4,H60*4,I60*3,J60*3,K60*3,L60*2,M60*2,N60*2)/27,2)</f>
-        <v>6.07</v>
+        <v>5.96</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10312,10 +10303,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10332,7 +10323,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="10.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="8.67"/>
@@ -10462,7 +10453,7 @@
         <v>9</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>10</v>
@@ -10478,10 +10469,10 @@
       </c>
       <c r="O3" s="1" t="n">
         <f aca="false">ROUND(SUM(F3*4,G3*4,H3*4,I3*3,J3*3,K3*3,L3*2,M3*2,N3*2)/27,2)</f>
-        <v>6.89</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>6</v>
       </c>
@@ -10516,7 +10507,7 @@
         <v>9</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M4" s="1" t="n">
         <v>5</v>
@@ -10526,10 +10517,10 @@
       </c>
       <c r="O4" s="1" t="n">
         <f aca="false">ROUND(SUM(F4*4,G4*4,H4*4,I4*3,J4*3,K4*3,L4*2,M4*2,N4*2)/27,2)</f>
-        <v>6.89</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.81</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>6</v>
       </c>
@@ -10546,7 +10537,7 @@
         <v>384</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>7</v>
@@ -10564,7 +10555,7 @@
         <v>7</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M5" s="1" t="n">
         <v>9</v>
@@ -10574,10 +10565,10 @@
       </c>
       <c r="O5" s="1" t="n">
         <f aca="false">ROUND(SUM(F5*4,G5*4,H5*4,I5*3,J5*3,K5*3,L5*2,M5*2,N5*2)/27,2)</f>
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>6</v>
       </c>
@@ -10600,7 +10591,7 @@
         <v>9</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>7</v>
@@ -10612,20 +10603,20 @@
         <v>4</v>
       </c>
       <c r="L6" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M6" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N6" s="1" t="n">
         <v>9</v>
       </c>
       <c r="O6" s="1" t="n">
         <f aca="false">ROUND(SUM(F6*4,G6*4,H6*4,I6*3,J6*3,K6*3,L6*2,M6*2,N6*2)/27,2)</f>
-        <v>6.96</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.63</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
@@ -10657,23 +10648,23 @@
         <v>6</v>
       </c>
       <c r="K7" s="1" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M7" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N7" s="1" t="n">
         <v>9</v>
       </c>
       <c r="O7" s="1" t="n">
         <f aca="false">ROUND(SUM(F7*4,G7*4,H7*4,I7*3,J7*3,K7*3,L7*2,M7*2,N7*2)/27,2)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
@@ -10690,7 +10681,7 @@
         <v>387</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>5</v>
@@ -10708,7 +10699,7 @@
         <v>9</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M8" s="1" t="n">
         <v>4</v>
@@ -10718,10 +10709,10 @@
       </c>
       <c r="O8" s="1" t="n">
         <f aca="false">ROUND(SUM(F8*4,G8*4,H8*4,I8*3,J8*3,K8*3,L8*2,M8*2,N8*2)/27,2)</f>
-        <v>7.63</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.33</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>6</v>
       </c>
@@ -10756,20 +10747,20 @@
         <v>7</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="M9" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N9" s="1" t="n">
         <v>4</v>
       </c>
       <c r="O9" s="1" t="n">
         <f aca="false">ROUND(SUM(F9*4,G9*4,H9*4,I9*3,J9*3,K9*3,L9*2,M9*2,N9*2)/27,2)</f>
-        <v>7.19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.52</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>6</v>
       </c>
@@ -10798,13 +10789,13 @@
         <v>8</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="K10" s="1" t="n">
         <v>6</v>
       </c>
       <c r="L10" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M10" s="1" t="n">
         <v>9</v>
@@ -10814,10 +10805,10 @@
       </c>
       <c r="O10" s="1" t="n">
         <f aca="false">ROUND(SUM(F10*4,G10*4,H10*4,I10*3,J10*3,K10*3,L10*2,M10*2,N10*2)/27,2)</f>
-        <v>7.59</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>6</v>
       </c>
@@ -10834,7 +10825,7 @@
         <v>40</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G11" s="1" t="n">
         <v>0</v>
@@ -10855,17 +10846,17 @@
         <v>5</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="N11" s="1" t="n">
         <v>10</v>
       </c>
       <c r="O11" s="1" t="n">
         <f aca="false">ROUND(SUM(F11*4,G11*4,H11*4,I11*3,J11*3,K11*3,L11*2,M11*2,N11*2)/27,2)</f>
-        <v>5.07</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4.11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>6</v>
       </c>
@@ -10891,7 +10882,7 @@
         <v>10</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J12" s="1" t="n">
         <v>6</v>
@@ -10903,17 +10894,17 @@
         <v>5</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N12" s="1" t="n">
         <v>4</v>
       </c>
       <c r="O12" s="1" t="n">
         <f aca="false">ROUND(SUM(F12*4,G12*4,H12*4,I12*3,J12*3,K12*3,L12*2,M12*2,N12*2)/27,2)</f>
-        <v>5.81</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>6</v>
       </c>
@@ -10939,29 +10930,29 @@
         <v>5</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J13" s="1" t="n">
         <v>6</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L13" s="1" t="n">
         <v>4</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="O13" s="1" t="n">
         <f aca="false">ROUND(SUM(F13*4,G13*4,H13*4,I13*3,J13*3,K13*3,L13*2,M13*2,N13*2)/27,2)</f>
-        <v>4.67</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.48</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>6</v>
       </c>
@@ -10981,13 +10972,13 @@
         <v>4</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>7</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J14" s="1" t="n">
         <v>9</v>
@@ -10996,7 +10987,7 @@
         <v>9</v>
       </c>
       <c r="L14" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M14" s="1" t="n">
         <v>10</v>
@@ -11006,10 +10997,10 @@
       </c>
       <c r="O14" s="1" t="n">
         <f aca="false">ROUND(SUM(F14*4,G14*4,H14*4,I14*3,J14*3,K14*3,L14*2,M14*2,N14*2)/27,2)</f>
-        <v>6.67</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.41</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>6</v>
       </c>
@@ -11035,7 +11026,7 @@
         <v>6</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J15" s="1" t="n">
         <v>6</v>
@@ -11054,10 +11045,10 @@
       </c>
       <c r="O15" s="1" t="n">
         <f aca="false">ROUND(SUM(F15*4,G15*4,H15*4,I15*3,J15*3,K15*3,L15*2,M15*2,N15*2)/27,2)</f>
-        <v>6.63</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>6</v>
       </c>
@@ -11080,13 +11071,13 @@
         <v>10</v>
       </c>
       <c r="H16" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J16" s="1" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="K16" s="1" t="n">
         <v>6</v>
@@ -11102,10 +11093,10 @@
       </c>
       <c r="O16" s="1" t="n">
         <f aca="false">ROUND(SUM(F16*4,G16*4,H16*4,I16*3,J16*3,K16*3,L16*2,M16*2,N16*2)/27,2)</f>
-        <v>7.11</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.59</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>6</v>
       </c>
@@ -11128,10 +11119,10 @@
         <v>8</v>
       </c>
       <c r="H17" s="1" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J17" s="1" t="n">
         <v>8</v>
@@ -11150,10 +11141,10 @@
       </c>
       <c r="O17" s="1" t="n">
         <f aca="false">ROUND(SUM(F17*4,G17*4,H17*4,I17*3,J17*3,K17*3,L17*2,M17*2,N17*2)/27,2)</f>
-        <v>6.59</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.63</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>6</v>
       </c>
@@ -11176,10 +11167,10 @@
         <v>8</v>
       </c>
       <c r="H18" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J18" s="1" t="n">
         <v>8</v>
@@ -11198,10 +11189,10 @@
       </c>
       <c r="O18" s="1" t="n">
         <f aca="false">ROUND(SUM(F18*4,G18*4,H18*4,I18*3,J18*3,K18*3,L18*2,M18*2,N18*2)/27,2)</f>
-        <v>7.04</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.52</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>6</v>
       </c>
@@ -11218,16 +11209,16 @@
         <v>396</v>
       </c>
       <c r="F19" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" s="1" t="n">
         <v>9</v>
       </c>
       <c r="H19" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J19" s="1" t="n">
         <v>9</v>
@@ -11236,7 +11227,7 @@
         <v>8</v>
       </c>
       <c r="L19" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M19" s="1" t="n">
         <v>5</v>
@@ -11246,7 +11237,7 @@
       </c>
       <c r="O19" s="1" t="n">
         <f aca="false">ROUND(SUM(F19*4,G19*4,H19*4,I19*3,J19*3,K19*3,L19*2,M19*2,N19*2)/27,2)</f>
-        <v>7.7</v>
+        <v>7.74</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11266,7 +11257,7 @@
         <v>397</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G20" s="1" t="n">
         <v>10</v>
@@ -11294,10 +11285,10 @@
       </c>
       <c r="O20" s="1" t="n">
         <f aca="false">ROUND(SUM(F20*4,G20*4,H20*4,I20*3,J20*3,K20*3,L20*2,M20*2,N20*2)/27,2)</f>
-        <v>9.44</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9.3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>6</v>
       </c>
@@ -11314,13 +11305,13 @@
         <v>398</v>
       </c>
       <c r="F21" s="1" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G21" s="1" t="n">
         <v>4</v>
       </c>
       <c r="H21" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I21" s="1" t="n">
         <v>0</v>
@@ -11342,10 +11333,10 @@
       </c>
       <c r="O21" s="1" t="n">
         <f aca="false">ROUND(SUM(F21*4,G21*4,H21*4,I21*3,J21*3,K21*3,L21*2,M21*2,N21*2)/27,2)</f>
-        <v>4.93</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.81</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>6</v>
       </c>
@@ -11362,7 +11353,7 @@
         <v>399</v>
       </c>
       <c r="F22" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G22" s="1" t="n">
         <v>9</v>
@@ -11390,10 +11381,10 @@
       </c>
       <c r="O22" s="1" t="n">
         <f aca="false">ROUND(SUM(F22*4,G22*4,H22*4,I22*3,J22*3,K22*3,L22*2,M22*2,N22*2)/27,2)</f>
-        <v>7.96</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.67</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>6</v>
       </c>
@@ -11410,19 +11401,19 @@
         <v>400</v>
       </c>
       <c r="F23" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G23" s="1" t="n">
         <v>10</v>
       </c>
       <c r="H23" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I23" s="1" t="n">
         <v>6</v>
       </c>
       <c r="J23" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K23" s="1" t="n">
         <v>9</v>
@@ -11438,10 +11429,10 @@
       </c>
       <c r="O23" s="1" t="n">
         <f aca="false">ROUND(SUM(F23*4,G23*4,H23*4,I23*3,J23*3,K23*3,L23*2,M23*2,N23*2)/27,2)</f>
-        <v>8.44</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.81</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>6</v>
       </c>
@@ -11458,7 +11449,7 @@
         <v>401</v>
       </c>
       <c r="F24" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G24" s="1" t="n">
         <v>7</v>
@@ -11486,10 +11477,10 @@
       </c>
       <c r="O24" s="1" t="n">
         <f aca="false">ROUND(SUM(F24*4,G24*4,H24*4,I24*3,J24*3,K24*3,L24*2,M24*2,N24*2)/27,2)</f>
-        <v>6.89</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>6</v>
       </c>
@@ -11506,7 +11497,7 @@
         <v>402</v>
       </c>
       <c r="F25" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G25" s="1" t="n">
         <v>8</v>
@@ -11534,7 +11525,7 @@
       </c>
       <c r="O25" s="1" t="n">
         <f aca="false">ROUND(SUM(F25*4,G25*4,H25*4,I25*3,J25*3,K25*3,L25*2,M25*2,N25*2)/27,2)</f>
-        <v>7.22</v>
+        <v>6.93</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11578,11 +11569,11 @@
         <v>8</v>
       </c>
       <c r="N26" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O26" s="1" t="n">
         <f aca="false">ROUND(SUM(F26*4,G26*4,H26*4,I26*3,J26*3,K26*3,L26*2,M26*2,N26*2)/27,2)</f>
-        <v>9</v>
+        <v>8.78</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11605,7 +11596,7 @@
         <v>7</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>10</v>
@@ -11626,11 +11617,11 @@
         <v>0</v>
       </c>
       <c r="N27" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O27" s="1" t="n">
         <f aca="false">ROUND(SUM(F27*4,G27*4,H27*4,I27*3,J27*3,K27*3,L27*2,M27*2,N27*2)/27,2)</f>
-        <v>7.67</v>
+        <v>8.26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11650,7 +11641,7 @@
         <v>405</v>
       </c>
       <c r="F28" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G28" s="1" t="n">
         <v>8</v>
@@ -11662,7 +11653,7 @@
         <v>9</v>
       </c>
       <c r="J28" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K28" s="1" t="n">
         <v>9</v>
@@ -11673,12 +11664,12 @@
       <c r="M28" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="N28" s="2" t="n">
-        <v>7</v>
+      <c r="N28" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="O28" s="1" t="n">
         <f aca="false">ROUND(SUM(F28*4,G28*4,H28*4,I28*3,J28*3,K28*3,L28*2,M28*2,N28*2)/27,2)</f>
-        <v>6.81</v>
+        <v>5.85</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11698,7 +11689,7 @@
         <v>406</v>
       </c>
       <c r="F29" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G29" s="1" t="n">
         <v>0</v>
@@ -11710,10 +11701,10 @@
         <v>9</v>
       </c>
       <c r="J29" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K29" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L29" s="1" t="n">
         <v>5</v>
@@ -11722,14 +11713,14 @@
         <v>9</v>
       </c>
       <c r="N29" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O29" s="1" t="n">
         <f aca="false">ROUND(SUM(F29*4,G29*4,H29*4,I29*3,J29*3,K29*3,L29*2,M29*2,N29*2)/27,2)</f>
-        <v>5.44</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.48</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>6</v>
       </c>
@@ -11746,7 +11737,7 @@
         <v>407</v>
       </c>
       <c r="F30" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G30" s="1" t="n">
         <v>6</v>
@@ -11758,10 +11749,10 @@
         <v>9</v>
       </c>
       <c r="J30" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K30" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L30" s="1" t="n">
         <v>5</v>
@@ -11770,14 +11761,14 @@
         <v>6</v>
       </c>
       <c r="N30" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O30" s="1" t="n">
         <f aca="false">ROUND(SUM(F30*4,G30*4,H30*4,I30*3,J30*3,K30*3,L30*2,M30*2,N30*2)/27,2)</f>
-        <v>5.78</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>6</v>
       </c>
@@ -11794,7 +11785,7 @@
         <v>408</v>
       </c>
       <c r="F31" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G31" s="1" t="n">
         <v>9</v>
@@ -11806,10 +11797,10 @@
         <v>6</v>
       </c>
       <c r="J31" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K31" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L31" s="1" t="n">
         <v>9</v>
@@ -11818,14 +11809,14 @@
         <v>7</v>
       </c>
       <c r="N31" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O31" s="1" t="n">
         <f aca="false">ROUND(SUM(F31*4,G31*4,H31*4,I31*3,J31*3,K31*3,L31*2,M31*2,N31*2)/27,2)</f>
-        <v>6.07</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.96</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>6</v>
       </c>
@@ -11842,10 +11833,10 @@
         <v>409</v>
       </c>
       <c r="F32" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G32" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H32" s="1" t="n">
         <v>4</v>
@@ -11854,10 +11845,10 @@
         <v>8</v>
       </c>
       <c r="J32" s="1" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K32" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L32" s="1" t="n">
         <v>9</v>
@@ -11866,14 +11857,14 @@
         <v>0</v>
       </c>
       <c r="N32" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O32" s="1" t="n">
         <f aca="false">ROUND(SUM(F32*4,G32*4,H32*4,I32*3,J32*3,K32*3,L32*2,M32*2,N32*2)/27,2)</f>
-        <v>6.74</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.63</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>6</v>
       </c>
@@ -11890,7 +11881,7 @@
         <v>410</v>
       </c>
       <c r="F33" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G33" s="1" t="n">
         <v>8</v>
@@ -11902,10 +11893,10 @@
         <v>9</v>
       </c>
       <c r="J33" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K33" s="1" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L33" s="1" t="n">
         <v>9</v>
@@ -11914,14 +11905,14 @@
         <v>8</v>
       </c>
       <c r="N33" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O33" s="1" t="n">
         <f aca="false">ROUND(SUM(F33*4,G33*4,H33*4,I33*3,J33*3,K33*3,L33*2,M33*2,N33*2)/27,2)</f>
-        <v>8.41</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.93</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>6</v>
       </c>
@@ -11950,10 +11941,10 @@
         <v>7</v>
       </c>
       <c r="J34" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K34" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L34" s="1" t="n">
         <v>8</v>
@@ -11966,10 +11957,10 @@
       </c>
       <c r="O34" s="1" t="n">
         <f aca="false">ROUND(SUM(F34*4,G34*4,H34*4,I34*3,J34*3,K34*3,L34*2,M34*2,N34*2)/27,2)</f>
-        <v>7.41</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>6</v>
       </c>
@@ -11998,7 +11989,7 @@
         <v>8</v>
       </c>
       <c r="J35" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K35" s="1" t="n">
         <v>6</v>
@@ -12014,10 +12005,10 @@
       </c>
       <c r="O35" s="1" t="n">
         <f aca="false">ROUND(SUM(F35*4,G35*4,H35*4,I35*3,J35*3,K35*3,L35*2,M35*2,N35*2)/27,2)</f>
-        <v>7.85</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.52</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>6</v>
       </c>
@@ -12034,7 +12025,7 @@
         <v>141</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G36" s="1" t="n">
         <v>10</v>
@@ -12049,7 +12040,7 @@
         <v>8</v>
       </c>
       <c r="K36" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L36" s="1" t="n">
         <v>4</v>
@@ -12062,10 +12053,10 @@
       </c>
       <c r="O36" s="1" t="n">
         <f aca="false">ROUND(SUM(F36*4,G36*4,H36*4,I36*3,J36*3,K36*3,L36*2,M36*2,N36*2)/27,2)</f>
-        <v>7.15</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.26</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <v>6</v>
       </c>
@@ -12082,7 +12073,7 @@
         <v>413</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>4</v>
@@ -12110,10 +12101,10 @@
       </c>
       <c r="O37" s="1" t="n">
         <f aca="false">ROUND(SUM(F37*4,G37*4,H37*4,I37*3,J37*3,K37*3,L37*2,M37*2,N37*2)/27,2)</f>
-        <v>6.11</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.37</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <v>6</v>
       </c>
@@ -12130,7 +12121,7 @@
         <v>414</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G38" s="1" t="n">
         <v>8</v>
@@ -12158,10 +12149,10 @@
       </c>
       <c r="O38" s="1" t="n">
         <f aca="false">ROUND(SUM(F38*4,G38*4,H38*4,I38*3,J38*3,K38*3,L38*2,M38*2,N38*2)/27,2)</f>
-        <v>6.37</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.52</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>6</v>
       </c>
@@ -12178,7 +12169,7 @@
         <v>415</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G39" s="1" t="n">
         <v>8</v>
@@ -12206,10 +12197,10 @@
       </c>
       <c r="O39" s="1" t="n">
         <f aca="false">ROUND(SUM(F39*4,G39*4,H39*4,I39*3,J39*3,K39*3,L39*2,M39*2,N39*2)/27,2)</f>
-        <v>6.63</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.93</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>6</v>
       </c>
@@ -12226,10 +12217,10 @@
         <v>416</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G40" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H40" s="1" t="n">
         <v>7</v>
@@ -12254,10 +12245,10 @@
       </c>
       <c r="O40" s="1" t="n">
         <f aca="false">ROUND(SUM(F40*4,G40*4,H40*4,I40*3,J40*3,K40*3,L40*2,M40*2,N40*2)/27,2)</f>
-        <v>5.93</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.63</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <v>6</v>
       </c>
@@ -12277,7 +12268,7 @@
         <v>9</v>
       </c>
       <c r="G41" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H41" s="1" t="n">
         <v>10</v>
@@ -12302,10 +12293,10 @@
       </c>
       <c r="O41" s="1" t="n">
         <f aca="false">ROUND(SUM(F41*4,G41*4,H41*4,I41*3,J41*3,K41*3,L41*2,M41*2,N41*2)/27,2)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>6</v>
       </c>
@@ -12322,10 +12313,10 @@
         <v>418</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G42" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H42" s="1" t="n">
         <v>9</v>
@@ -12350,10 +12341,10 @@
       </c>
       <c r="O42" s="1" t="n">
         <f aca="false">ROUND(SUM(F42*4,G42*4,H42*4,I42*3,J42*3,K42*3,L42*2,M42*2,N42*2)/27,2)</f>
-        <v>7.93</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.48</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>6</v>
       </c>
@@ -12373,7 +12364,7 @@
         <v>10</v>
       </c>
       <c r="G43" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H43" s="1" t="n">
         <v>7</v>
@@ -12398,10 +12389,10 @@
       </c>
       <c r="O43" s="1" t="n">
         <f aca="false">ROUND(SUM(F43*4,G43*4,H43*4,I43*3,J43*3,K43*3,L43*2,M43*2,N43*2)/27,2)</f>
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.85</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <v>6</v>
       </c>
@@ -12421,7 +12412,7 @@
         <v>9</v>
       </c>
       <c r="G44" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H44" s="1" t="n">
         <v>7</v>
@@ -12446,10 +12437,10 @@
       </c>
       <c r="O44" s="1" t="n">
         <f aca="false">ROUND(SUM(F44*4,G44*4,H44*4,I44*3,J44*3,K44*3,L44*2,M44*2,N44*2)/27,2)</f>
-        <v>7.26</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.96</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <v>6</v>
       </c>
@@ -12466,7 +12457,7 @@
         <v>421</v>
       </c>
       <c r="F45" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G45" s="1" t="n">
         <v>8</v>
@@ -12494,10 +12485,10 @@
       </c>
       <c r="O45" s="1" t="n">
         <f aca="false">ROUND(SUM(F45*4,G45*4,H45*4,I45*3,J45*3,K45*3,L45*2,M45*2,N45*2)/27,2)</f>
-        <v>6.81</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.07</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <v>6</v>
       </c>
@@ -12514,7 +12505,7 @@
         <v>422</v>
       </c>
       <c r="F46" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G46" s="1" t="n">
         <v>8</v>
@@ -12542,10 +12533,10 @@
       </c>
       <c r="O46" s="1" t="n">
         <f aca="false">ROUND(SUM(F46*4,G46*4,H46*4,I46*3,J46*3,K46*3,L46*2,M46*2,N46*2)/27,2)</f>
-        <v>8.56</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8.7</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <v>6</v>
       </c>
@@ -12562,7 +12553,7 @@
         <v>423</v>
       </c>
       <c r="F47" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G47" s="1" t="n">
         <v>5</v>
@@ -12590,10 +12581,10 @@
       </c>
       <c r="O47" s="1" t="n">
         <f aca="false">ROUND(SUM(F47*4,G47*4,H47*4,I47*3,J47*3,K47*3,L47*2,M47*2,N47*2)/27,2)</f>
-        <v>7.15</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.85</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>6</v>
       </c>
@@ -12610,7 +12601,7 @@
         <v>424</v>
       </c>
       <c r="F48" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G48" s="1" t="n">
         <v>5</v>
@@ -12638,10 +12629,10 @@
       </c>
       <c r="O48" s="1" t="n">
         <f aca="false">ROUND(SUM(F48*4,G48*4,H48*4,I48*3,J48*3,K48*3,L48*2,M48*2,N48*2)/27,2)</f>
-        <v>7.74</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>6</v>
       </c>
@@ -12658,7 +12649,7 @@
         <v>425</v>
       </c>
       <c r="F49" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G49" s="1" t="n">
         <v>5</v>
@@ -12686,10 +12677,10 @@
       </c>
       <c r="O49" s="1" t="n">
         <f aca="false">ROUND(SUM(F49*4,G49*4,H49*4,I49*3,J49*3,K49*3,L49*2,M49*2,N49*2)/27,2)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8.15</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>6</v>
       </c>
@@ -12706,7 +12697,7 @@
         <v>426</v>
       </c>
       <c r="F50" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G50" s="1" t="n">
         <v>5</v>
@@ -12734,10 +12725,10 @@
       </c>
       <c r="O50" s="1" t="n">
         <f aca="false">ROUND(SUM(F50*4,G50*4,H50*4,I50*3,J50*3,K50*3,L50*2,M50*2,N50*2)/27,2)</f>
-        <v>5.52</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.81</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
         <v>6</v>
       </c>
@@ -12754,7 +12745,7 @@
         <v>427</v>
       </c>
       <c r="F51" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G51" s="1" t="n">
         <v>5</v>
@@ -12782,10 +12773,10 @@
       </c>
       <c r="O51" s="1" t="n">
         <f aca="false">ROUND(SUM(F51*4,G51*4,H51*4,I51*3,J51*3,K51*3,L51*2,M51*2,N51*2)/27,2)</f>
-        <v>6.96</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.81</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
         <v>6</v>
       </c>
@@ -12802,7 +12793,7 @@
         <v>428</v>
       </c>
       <c r="F52" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G52" s="1" t="n">
         <v>5</v>
@@ -12830,10 +12821,10 @@
       </c>
       <c r="O52" s="1" t="n">
         <f aca="false">ROUND(SUM(F52*4,G52*4,H52*4,I52*3,J52*3,K52*3,L52*2,M52*2,N52*2)/27,2)</f>
-        <v>5.19</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.33</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <v>6</v>
       </c>
@@ -12850,7 +12841,7 @@
         <v>429</v>
       </c>
       <c r="F53" s="1" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G53" s="1" t="n">
         <v>6</v>
@@ -12878,10 +12869,10 @@
       </c>
       <c r="O53" s="1" t="n">
         <f aca="false">ROUND(SUM(F53*4,G53*4,H53*4,I53*3,J53*3,K53*3,L53*2,M53*2,N53*2)/27,2)</f>
-        <v>7.81</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.93</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
         <v>6</v>
       </c>
@@ -12898,7 +12889,7 @@
         <v>330</v>
       </c>
       <c r="F54" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G54" s="1" t="n">
         <v>6</v>
@@ -12926,10 +12917,10 @@
       </c>
       <c r="O54" s="1" t="n">
         <f aca="false">ROUND(SUM(F54*4,G54*4,H54*4,I54*3,J54*3,K54*3,L54*2,M54*2,N54*2)/27,2)</f>
-        <v>7.89</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7.74</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <v>6</v>
       </c>
@@ -12946,7 +12937,7 @@
         <v>328</v>
       </c>
       <c r="F55" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G55" s="1" t="n">
         <v>6</v>
@@ -12974,10 +12965,10 @@
       </c>
       <c r="O55" s="1" t="n">
         <f aca="false">ROUND(SUM(F55*4,G55*4,H55*4,I55*3,J55*3,K55*3,L55*2,M55*2,N55*2)/27,2)</f>
-        <v>6.63</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.48</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <v>6</v>
       </c>
@@ -12994,7 +12985,7 @@
         <v>430</v>
       </c>
       <c r="F56" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G56" s="1" t="n">
         <v>0</v>
@@ -13022,10 +13013,10 @@
       </c>
       <c r="O56" s="1" t="n">
         <f aca="false">ROUND(SUM(F56*4,G56*4,H56*4,I56*3,J56*3,K56*3,L56*2,M56*2,N56*2)/27,2)</f>
-        <v>6.37</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5.93</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
         <v>6</v>
       </c>
@@ -13073,7 +13064,7 @@
         <v>7.52</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
         <v>6</v>
       </c>
@@ -13090,7 +13081,7 @@
         <v>354</v>
       </c>
       <c r="F58" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G58" s="1" t="n">
         <v>8</v>
@@ -13118,10 +13109,10 @@
       </c>
       <c r="O58" s="1" t="n">
         <f aca="false">ROUND(SUM(F58*4,G58*4,H58*4,I58*3,J58*3,K58*3,L58*2,M58*2,N58*2)/27,2)</f>
-        <v>8.33</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8.48</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
         <v>6</v>
       </c>
@@ -13169,7 +13160,7 @@
         <v>7.56</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
         <v>6</v>
       </c>
@@ -13186,7 +13177,7 @@
         <v>372</v>
       </c>
       <c r="F60" s="1" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G60" s="1" t="n">
         <v>5</v>
@@ -13214,10 +13205,10 @@
       </c>
       <c r="O60" s="1" t="n">
         <f aca="false">ROUND(SUM(F60*4,G60*4,H60*4,I60*3,J60*3,K60*3,L60*2,M60*2,N60*2)/27,2)</f>
-        <v>5.44</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.48</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
         <v>6</v>
       </c>
@@ -13234,7 +13225,7 @@
         <v>433</v>
       </c>
       <c r="F61" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G61" s="1" t="n">
         <v>8</v>
@@ -13262,9 +13253,15 @@
       </c>
       <c r="O61" s="1" t="n">
         <f aca="false">ROUND(SUM(F61*4,G61*4,H61*4,I61*3,J61*3,K61*3,L61*2,M61*2,N61*2)/27,2)</f>
-        <v>6.81</v>
-      </c>
-    </row>
+        <v>6.96</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>